<commit_message>
Atualização dos artefatos para AC 5
</commit_message>
<xml_diff>
--- a/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/17. Análise dos Eventos para cada Cenário.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elton\Desktop\OPE\OPE_Artefatos_HAIR2U\Agendar servicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elton\Desktop\OPE\OPE_Artefatos_HAIR2U\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E834393-6635-4BE6-AB57-58FFD5065255}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10C132A-5B48-45ED-B3BE-8C188CB8AB0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40935" yWindow="4545" windowWidth="18060" windowHeight="9180" xr2:uid="{C877A977-5D9B-4F08-BA96-DC6508DF2181}"/>
+    <workbookView xWindow="-28320" yWindow="4950" windowWidth="17280" windowHeight="8400" xr2:uid="{C877A977-5D9B-4F08-BA96-DC6508DF2181}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>capacidade</t>
   </si>
@@ -87,20 +87,20 @@
     <t>Receber serviços</t>
   </si>
   <si>
-    <t>Cliente deseja um encaixe?</t>
-  </si>
-  <si>
-    <t>X(1)</t>
-  </si>
-  <si>
     <t>Cliente solicita o serviço</t>
+  </si>
+  <si>
+    <t>Cliente solicita a troca do produto</t>
+  </si>
+  <si>
+    <t>Trocar produtos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,22 +118,14 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,8 +168,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -250,11 +248,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -284,6 +295,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -292,43 +354,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -715,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A3E32E-1996-41D2-AF64-2CDCA275956E}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,26 +767,26 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="16"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -782,8 +809,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="31" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="11">
@@ -802,8 +829,8 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="11">
         <v>2</v>
       </c>
@@ -820,7 +847,7 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
@@ -832,109 +859,86 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="21">
         <v>4</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
+    </row>
+    <row r="8" spans="1:10" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="B8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="17">
+        <v>5</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24">
-        <v>5</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="15">
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="D8:D9"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>